<commit_message>
Modified test raport, tried to make video automatic change work
</commit_message>
<xml_diff>
--- a/Digital_Signage_kayttajatestaus.xlsx
+++ b/Digital_Signage_kayttajatestaus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HannaHoffren/Desktop/Koulu/Webteknologiat ja media-alustat/Javascript/DSdemo/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HannaHoffren/Desktop/Koulu/Webteknologiat ja media-alustat/Javascript/DSdemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D015FA7-E516-194A-A072-8A0BE6268B13}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CC16C7-A967-2847-90B5-F57F12092FE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="460" windowWidth="26260" windowHeight="17040" activeTab="3" xr2:uid="{79DCB777-8955-9D47-80BA-343B61CB2576}"/>
+    <workbookView xWindow="2160" yWindow="460" windowWidth="26260" windowHeight="17040" xr2:uid="{79DCB777-8955-9D47-80BA-343B61CB2576}"/>
   </bookViews>
   <sheets>
     <sheet name="Myyrmäki" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="54">
   <si>
     <t>Stepit</t>
   </si>
@@ -175,6 +175,27 @@
   </si>
   <si>
     <t>Slideshow jatkaa valitun toimipisteen tiedoilla pyörimistä siitä kohdasta mistä vaihto tapahtuu</t>
+  </si>
+  <si>
+    <t>Reittitiedot ovat oikein (Kellonaika näkyy oikein)</t>
+  </si>
+  <si>
+    <t>Sunnuntai = ei ruokalistaa</t>
+  </si>
+  <si>
+    <t>Videossa näkyy myyrmäen video</t>
+  </si>
+  <si>
+    <t>Oikeat tiedot haetaan omasta valitulla kielellä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Väärän toimipisteen video </t>
+  </si>
+  <si>
+    <t>Sunnuntaina ei ruokalistaa</t>
+  </si>
+  <si>
+    <t>Väärän toimipisteen video</t>
   </si>
 </sst>
 </file>
@@ -238,7 +259,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +294,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF73EC5E"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -316,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -345,6 +372,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,16 +689,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5199FA5F-FC79-9E4F-AE5A-4740C4DCB494}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
-    <col min="3" max="3" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="81.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -772,7 +800,9 @@
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -785,7 +815,9 @@
         <v>12</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -796,7 +828,9 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -806,10 +840,12 @@
         <v>32</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -821,8 +857,12 @@
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
@@ -835,7 +875,9 @@
         <v>13</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -848,7 +890,9 @@
         <v>8</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -861,7 +905,9 @@
         <v>10</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -874,7 +920,9 @@
         <v>11</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -884,7 +932,9 @@
         <v>35</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -897,7 +947,9 @@
         <v>46</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
@@ -936,7 +988,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,7 +996,7 @@
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1048,7 +1100,9 @@
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -1061,7 +1115,9 @@
         <v>43</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -1072,7 +1128,9 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -1085,7 +1143,9 @@
         <v>33</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -1097,8 +1157,12 @@
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
@@ -1111,7 +1175,9 @@
         <v>13</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -1124,7 +1190,9 @@
         <v>8</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -1136,8 +1204,12 @@
       <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -1150,7 +1222,9 @@
         <v>11</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -1160,7 +1234,9 @@
         <v>35</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -1173,7 +1249,9 @@
         <v>46</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1185,7 +1263,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1193,7 +1271,7 @@
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1297,7 +1375,9 @@
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -1310,7 +1390,9 @@
         <v>42</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -1323,7 +1405,9 @@
         <v>39</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
@@ -1334,7 +1418,9 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -1344,10 +1430,12 @@
         <v>32</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="17">
@@ -1359,8 +1447,12 @@
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -1370,10 +1462,12 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="17">
@@ -1386,7 +1480,9 @@
         <v>8</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -1398,8 +1494,12 @@
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
@@ -1412,7 +1512,9 @@
         <v>11</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -1422,7 +1524,9 @@
         <v>35</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="17">
@@ -1435,7 +1539,9 @@
         <v>46</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1446,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F672E712-BF14-8D46-BAA8-BB5CA741EB5A}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1455,7 +1561,7 @@
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1559,7 +1665,9 @@
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -1572,7 +1680,9 @@
         <v>44</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -1583,7 +1693,9 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -1596,7 +1708,9 @@
         <v>33</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -1609,7 +1723,9 @@
         <v>6</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
@@ -1622,7 +1738,9 @@
         <v>13</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -1635,7 +1753,9 @@
         <v>8</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -1647,8 +1767,12 @@
       <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -1661,7 +1785,9 @@
         <v>11</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -1671,7 +1797,9 @@
         <v>35</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -1684,7 +1812,9 @@
         <v>46</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixes header font and upload error images
</commit_message>
<xml_diff>
--- a/Digital_Signage_kayttajatestaus.xlsx
+++ b/Digital_Signage_kayttajatestaus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HannaHoffren/Desktop/Koulu/Webteknologiat ja media-alustat/Javascript/DSdemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5F057D-0D1D-C248-9B81-B5D7D1C3C997}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8510C1CF-BEFB-8F46-9936-289EE8F2ED0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="460" windowWidth="26260" windowHeight="17040" activeTab="2" xr2:uid="{79DCB777-8955-9D47-80BA-343B61CB2576}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="47">
   <si>
     <t>Stepit</t>
   </si>
@@ -164,13 +164,16 @@
     <t>Reittitiedot ovat oikein (Kellonaika näkyy oikein)</t>
   </si>
   <si>
-    <t>Sunnuntai = ei ruokalistaa</t>
-  </si>
-  <si>
     <t>Oikeat tiedot haetaan omasta valitulla kielellä</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Oikeanlainen virheilmoitus näkyy</t>
+  </si>
+  <si>
+    <t>Ruokalista ei näy</t>
   </si>
 </sst>
 </file>
@@ -684,7 +687,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,7 +738,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -847,11 +850,9 @@
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>22</v>
+      <c r="D18" s="1"/>
+      <c r="E18" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -978,7 +979,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1016,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
@@ -1140,10 +1141,10 @@
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>22</v>
+        <v>46</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1243,7 +1244,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,7 +1281,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
@@ -1419,11 +1420,9 @@
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>22</v>
+      <c r="D19" s="22"/>
+      <c r="E19" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1434,7 +1433,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="12" t="s">
@@ -1523,7 +1522,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1531,7 +1530,7 @@
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1560,7 +1559,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
@@ -1685,7 +1684,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>22</v>

</xml_diff>